<commit_message>
Added checking for synchronized sensors
</commit_message>
<xml_diff>
--- a/Data/IoT enriched event log paper/tables/sensor_event_time_deltas.xlsx
+++ b/Data/IoT enriched event log paper/tables/sensor_event_time_deltas.xlsx
@@ -458,12 +458,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#CompressorPowerLevel</t>
+          <t>http://iot.uni-trier.de/FTOnto#LightBarrierInterrupted</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#OV_1_WT_1_Compressor_8</t>
+          <t>http://iot.uni-trier.de/FTOnto#OV_1_Light_Barrier_5</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -476,12 +476,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#PositionSwitchPressed</t>
+          <t>http://iot.uni-trier.de/StreamDataAnnotationOnto#OV_1_Property_Current_Task_Elapsed_Seconds_Since_Start</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#OV_1_Position_Switch_2</t>
+          <t>http://iot.uni-trier.de/FTOnto#OV_1</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -494,12 +494,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#LightBarrierInterrupted</t>
+          <t>http://iot.uni-trier.de/FTOnto#PositionSwitchPressed</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#OV_1_Light_Barrier_5</t>
+          <t>http://iot.uni-trier.de/FTOnto#OV_1_Position_Switch_2</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -512,12 +512,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#MotorSpeed</t>
+          <t>http://iot.uni-trier.de/FTOnto#ValveOpen</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#OV_1_Motor_1</t>
+          <t>http://iot.uni-trier.de/FTOnto#OV_1_Valve_7</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -530,12 +530,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#ValveOpen</t>
+          <t>http://iot.uni-trier.de/StreamDataAnnotationOnto#OV_1_Property_Current_State</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#OV_1_Valve_7</t>
+          <t>http://iot.uni-trier.de/FTOnto#OV_1</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -548,12 +548,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/StreamDataAnnotationOnto#OV_1_Property_Current_Task_Elapsed_Seconds_Since_Start</t>
+          <t>http://iot.uni-trier.de/FTOnto#PositionSwitchPressed</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#OV_1</t>
+          <t>http://iot.uni-trier.de/FTOnto#OV_1_Position_Switch_1</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -566,12 +566,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/StreamDataAnnotationOnto#OV_1_Property_Current_State</t>
+          <t>http://iot.uni-trier.de/FTOnto#MotorSpeed</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#OV_1</t>
+          <t>http://iot.uni-trier.de/FTOnto#OV_1_Motor_1</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -584,12 +584,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#PositionSwitchPressed</t>
+          <t>http://iot.uni-trier.de/FTOnto#CompressorPowerLevel</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>http://iot.uni-trier.de/FTOnto#OV_1_Position_Switch_1</t>
+          <t>http://iot.uni-trier.de/FTOnto#OV_1_WT_1_Compressor_8</t>
         </is>
       </c>
       <c r="C9" t="n">

</xml_diff>